<commit_message>
tentative gamm code (needs more thinking)
</commit_message>
<xml_diff>
--- a/RSFNT Study Protocol.xlsx
+++ b/RSFNT Study Protocol.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Text_Font\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\Text_Font\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A37497-412B-4480-BEDE-C66F0C0DDF0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +36,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>lang_use</t>
-  </si>
-  <si>
     <t>native</t>
   </si>
   <si>
@@ -142,12 +139,15 @@
   </si>
   <si>
     <t>LEFT EYE TRACKED/MAKE UP</t>
+  </si>
+  <si>
+    <t>lang_use_years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,20 +458,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="67.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -482,1554 +483,1554 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
         <v>13</v>
       </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
         <v>17</v>
       </c>
-      <c r="H14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20">
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29">
         <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30">
         <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32">
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <v>19</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34">
         <v>19</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H34" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35">
         <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" t="s">
         <v>23</v>
       </c>
-      <c r="G35" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36">
         <v>21</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37">
         <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39">
         <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40">
         <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41">
         <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H41" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42">
         <v>21</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C43">
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45">
         <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C47">
         <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G47" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" t="s">
         <v>29</v>
       </c>
-      <c r="H47" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C48">
         <v>19</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49">
         <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C50">
         <v>21</v>
       </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51">
         <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C52">
         <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C53">
         <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C54">
         <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H54" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55">
         <v>19</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C56">
         <v>21</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E56">
         <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C57">
         <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H57" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58">
         <v>22</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I58" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C59">
         <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I59" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C60">
         <v>21</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E60">
         <v>5.5</v>
       </c>
       <c r="F60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C61">
         <v>23</v>
       </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H61" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C62">
         <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H62" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C63">
         <v>19</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I63" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C64">
         <v>26</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E64">
         <v>6</v>
       </c>
       <c r="F64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I64" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C65">
         <v>19</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>